<commit_message>
Updated based on ETL
</commit_message>
<xml_diff>
--- a/Resources/Raw/Source_References.xlsx
+++ b/Resources/Raw/Source_References.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dhanu\Desktop\Analysis Project\Final Project\Final_Project-Group1\Resources\Raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1F8EDBB-636C-4A83-979C-61808BDA998E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC767B6F-E07F-433F-9D57-A135BFC60551}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -132,9 +132,6 @@
     <t>https://ourworldindata.org/cancer</t>
   </si>
   <si>
-    <t>https://data.worldbank.org/indicator/SH.ALC.PCAP.LI</t>
-  </si>
-  <si>
     <t xml:space="preserve">https://immunizationdata.who.int/pages/coverage/BCG.html?CODE=Global&amp;ANTIGEN=BCG </t>
   </si>
   <si>
@@ -198,9 +195,6 @@
     <t>Description</t>
   </si>
   <si>
-    <t>Total alcohol consumption per capita (liters of pure alcohol, projected estimates, 15+ years of age)</t>
-  </si>
-  <si>
     <t>WHO/UNICEF Joint Estimates of National Immunization Coverage (WUENIC) of BCG</t>
   </si>
   <si>
@@ -277,6 +271,12 @@
   </si>
   <si>
     <t>https://data.worldbank.org/indicator/NY.GDP.PCAP.KD.ZG</t>
+  </si>
+  <si>
+    <t>https://www.who.int/data/gho/data/indicators/indicator-details/GHO/alcohol-recorded-per-capita-(15-)-consumption-(in-litres-of-pure-alcohol)#:~:text=Definition%3A,sales%20data%20often%20via%20taxation.</t>
+  </si>
+  <si>
+    <t>Alcohol, recorded per capita (15+) consumption (in litres of pure alcohol)</t>
   </si>
 </sst>
 </file>
@@ -633,9 +633,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -656,7 +654,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -670,7 +668,7 @@
         <v>4</v>
       </c>
       <c r="D2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
@@ -684,7 +682,7 @@
         <v>32</v>
       </c>
       <c r="D3" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
@@ -696,7 +694,7 @@
         <v>34</v>
       </c>
       <c r="D4" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
@@ -707,10 +705,10 @@
         <v>7</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>35</v>
+        <v>82</v>
       </c>
       <c r="D5" t="s">
-        <v>57</v>
+        <v>83</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -722,7 +720,7 @@
         <v>33</v>
       </c>
       <c r="D6" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
@@ -733,10 +731,10 @@
         <v>12</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D7" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
@@ -745,10 +743,10 @@
         <v>13</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D8" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
@@ -757,10 +755,10 @@
         <v>14</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D9" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
@@ -769,10 +767,10 @@
         <v>15</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D10" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
@@ -783,10 +781,10 @@
         <v>18</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D11" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
@@ -795,10 +793,10 @@
         <v>19</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D12" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
@@ -807,10 +805,10 @@
         <v>20</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D13" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
@@ -819,10 +817,10 @@
         <v>21</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D14" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
@@ -833,10 +831,10 @@
         <v>23</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D15" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
@@ -845,22 +843,22 @@
         <v>24</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D16" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="5"/>
       <c r="B17" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D17" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
@@ -869,22 +867,22 @@
         <v>17</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D18" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="5"/>
       <c r="B19" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D19" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
@@ -895,10 +893,10 @@
         <v>26</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D20" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
@@ -907,22 +905,22 @@
         <v>27</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D21" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="5"/>
       <c r="B22" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D22" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
@@ -933,10 +931,10 @@
         <v>29</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D23" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
@@ -945,13 +943,13 @@
         <v>30</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D24" t="s">
+        <v>78</v>
+      </c>
+      <c r="E24" s="4" t="s">
         <v>80</v>
-      </c>
-      <c r="E24" s="4" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
@@ -960,10 +958,10 @@
         <v>31</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D25" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="E25" s="4"/>
     </row>
@@ -983,28 +981,27 @@
     <hyperlink ref="C3" r:id="rId2" xr:uid="{3A2534F6-5382-403B-A3BC-13C1A44E5200}"/>
     <hyperlink ref="C6" r:id="rId3" xr:uid="{CFD58E32-0EA6-4F7B-A483-C192AF3009BA}"/>
     <hyperlink ref="C4" r:id="rId4" xr:uid="{466F8AFE-FF4A-4B94-86A9-8CE925C7CBF0}"/>
-    <hyperlink ref="C5" r:id="rId5" xr:uid="{A6A5E8DD-B10E-48ED-AEA4-5332A95A7368}"/>
-    <hyperlink ref="C7" r:id="rId6" xr:uid="{99212F75-DCDE-49BB-8FA1-03831C529140}"/>
-    <hyperlink ref="C8" r:id="rId7" xr:uid="{A0254319-A83C-47DD-9278-32F6132225F7}"/>
-    <hyperlink ref="C9" r:id="rId8" xr:uid="{A8E7D092-2C7C-4033-9B31-ACC5748E751D}"/>
-    <hyperlink ref="C10" r:id="rId9" xr:uid="{0956841E-427E-43ED-BFB1-C41F919916D0}"/>
-    <hyperlink ref="C15" r:id="rId10" location=" " xr:uid="{E68CA478-1E1A-4AB0-88BD-23BA2616343A}"/>
-    <hyperlink ref="C16" r:id="rId11" xr:uid="{2E37B93B-977B-4E07-A1E9-12E88B660387}"/>
-    <hyperlink ref="C20" r:id="rId12" location=" " xr:uid="{0F46194F-30B0-4015-A79D-3446FEC57C4B}"/>
-    <hyperlink ref="C21" r:id="rId13" location=" " xr:uid="{FB024623-D02F-4955-BD55-6E88BD221822}"/>
-    <hyperlink ref="C22" r:id="rId14" location=" " xr:uid="{222848D8-AEC4-4429-95B9-B226B43F6CF7}"/>
-    <hyperlink ref="C14" r:id="rId15" xr:uid="{D4D2A64D-61AF-4BD0-96B4-DF0442D555E5}"/>
-    <hyperlink ref="C13" r:id="rId16" xr:uid="{247F742A-6140-48FF-8A79-B54CF57C86FE}"/>
-    <hyperlink ref="C12" r:id="rId17" xr:uid="{404923FC-E1CE-4AFD-8EC6-AC91EA2C6317}"/>
-    <hyperlink ref="C11" r:id="rId18" xr:uid="{B6415944-AFF4-4517-89B9-23AAC1CF1623}"/>
-    <hyperlink ref="C18" r:id="rId19" xr:uid="{C8AA1D66-480F-4329-9621-1BC012964869}"/>
-    <hyperlink ref="C17" r:id="rId20" xr:uid="{FDFE3A0A-27E6-4136-882E-7AD708EFF769}"/>
-    <hyperlink ref="C19" r:id="rId21" xr:uid="{4CBE2B26-E564-4C25-B5DA-4EF9540B2426}"/>
-    <hyperlink ref="C23" r:id="rId22" xr:uid="{6B8190DF-3677-4D24-AAB9-F0CF355B0754}"/>
-    <hyperlink ref="C24" r:id="rId23" xr:uid="{7E3B4A01-486B-4AB9-888A-7584084AD940}"/>
-    <hyperlink ref="C25" r:id="rId24" xr:uid="{8474A1C4-18EE-4E2E-81D0-39CF1B4738F0}"/>
+    <hyperlink ref="C7" r:id="rId5" xr:uid="{99212F75-DCDE-49BB-8FA1-03831C529140}"/>
+    <hyperlink ref="C8" r:id="rId6" xr:uid="{A0254319-A83C-47DD-9278-32F6132225F7}"/>
+    <hyperlink ref="C9" r:id="rId7" xr:uid="{A8E7D092-2C7C-4033-9B31-ACC5748E751D}"/>
+    <hyperlink ref="C10" r:id="rId8" xr:uid="{0956841E-427E-43ED-BFB1-C41F919916D0}"/>
+    <hyperlink ref="C15" r:id="rId9" location=" " xr:uid="{E68CA478-1E1A-4AB0-88BD-23BA2616343A}"/>
+    <hyperlink ref="C16" r:id="rId10" xr:uid="{2E37B93B-977B-4E07-A1E9-12E88B660387}"/>
+    <hyperlink ref="C20" r:id="rId11" location=" " xr:uid="{0F46194F-30B0-4015-A79D-3446FEC57C4B}"/>
+    <hyperlink ref="C21" r:id="rId12" location=" " xr:uid="{FB024623-D02F-4955-BD55-6E88BD221822}"/>
+    <hyperlink ref="C22" r:id="rId13" location=" " xr:uid="{222848D8-AEC4-4429-95B9-B226B43F6CF7}"/>
+    <hyperlink ref="C14" r:id="rId14" xr:uid="{D4D2A64D-61AF-4BD0-96B4-DF0442D555E5}"/>
+    <hyperlink ref="C13" r:id="rId15" xr:uid="{247F742A-6140-48FF-8A79-B54CF57C86FE}"/>
+    <hyperlink ref="C12" r:id="rId16" xr:uid="{404923FC-E1CE-4AFD-8EC6-AC91EA2C6317}"/>
+    <hyperlink ref="C11" r:id="rId17" xr:uid="{B6415944-AFF4-4517-89B9-23AAC1CF1623}"/>
+    <hyperlink ref="C18" r:id="rId18" xr:uid="{C8AA1D66-480F-4329-9621-1BC012964869}"/>
+    <hyperlink ref="C17" r:id="rId19" xr:uid="{FDFE3A0A-27E6-4136-882E-7AD708EFF769}"/>
+    <hyperlink ref="C19" r:id="rId20" xr:uid="{4CBE2B26-E564-4C25-B5DA-4EF9540B2426}"/>
+    <hyperlink ref="C23" r:id="rId21" xr:uid="{6B8190DF-3677-4D24-AAB9-F0CF355B0754}"/>
+    <hyperlink ref="C24" r:id="rId22" xr:uid="{7E3B4A01-486B-4AB9-888A-7584084AD940}"/>
+    <hyperlink ref="C25" r:id="rId23" xr:uid="{8474A1C4-18EE-4E2E-81D0-39CF1B4738F0}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId25"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId24"/>
 </worksheet>
 </file>
</xml_diff>